<commit_message>
Explore ORO_branch screening predictions -- something may be wrong because a very low number of inclusions
</commit_message>
<xml_diff>
--- a/data/derived-data/coding/variablePriorities.xlsx
+++ b/data/derived-data/coding/variablePriorities.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="81">
   <si>
     <t>Variable name</t>
   </si>
@@ -252,13 +252,19 @@
     <t>Intervention_0</t>
   </si>
   <si>
-    <t>ORO_branch used for screening, if not run first</t>
-  </si>
-  <si>
     <t>predict | Data == primary</t>
   </si>
   <si>
-    <t>predict oro_any | oro_branch; development stage for all</t>
+    <t>if ORO_branch used for screening then skip this cluster, if not, run together with Intervention_1 cluster</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>techological_scalability</t>
+  </si>
+  <si>
+    <t>technological_readiness</t>
   </si>
 </sst>
 </file>
@@ -287,7 +293,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,6 +318,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -325,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -336,6 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -633,7 +646,7 @@
     <col min="9" max="9" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,52 +666,52 @@
       <c r="H1" s="3"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="D2">
         <f>VLOOKUP(C2,F:F:G:G,2,FALSE)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B3">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D3">
         <f>VLOOKUP(C3,F:F:G:G,2,FALSE)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B4">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D4">
         <f>VLOOKUP(C4,F:F:G:G,2,FALSE)</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>68</v>
@@ -708,19 +721,19 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="D5">
         <f>VLOOKUP(C5,F:F:G:G,2,FALSE)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
         <v>69</v>
@@ -738,109 +751,106 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B6">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="D6">
         <f>VLOOKUP(C6,F:F:G:G,2,FALSE)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F6" t="s">
         <v>75</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="10">
         <v>0</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H16" si="0">COUNTIF(C:C,F6)</f>
+        <f>COUNTIF(C:C,F6)</f>
         <v>1</v>
       </c>
       <c r="I6" t="s">
         <v>56</v>
       </c>
       <c r="J6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="D7">
         <f>VLOOKUP(C7,F:F:G:G,2,FALSE)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
         <v>49</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="10">
         <v>1</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(C:C,F7)</f>
         <v>2</v>
       </c>
       <c r="I7" t="s">
         <v>56</v>
       </c>
-      <c r="J7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="D8">
         <f>VLOOKUP(C8,F:F:G:G,2,FALSE)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
         <v>26</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="10">
         <v>2</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(C:C,F8)</f>
         <v>5</v>
       </c>
       <c r="I8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="B9">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="D9">
         <f>VLOOKUP(C9,F:F:G:G,2,FALSE)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
         <v>51</v>
@@ -849,26 +859,26 @@
         <v>3</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(C:C,F9)</f>
         <v>2</v>
       </c>
       <c r="I9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B10">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D10">
         <f>VLOOKUP(C10,F:F:G:G,2,FALSE)</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
@@ -877,26 +887,26 @@
         <v>4</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(C:C,F10)</f>
         <v>6</v>
       </c>
       <c r="I10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D11">
         <f>VLOOKUP(C11,F:F:G:G,2,FALSE)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
         <v>59</v>
@@ -905,26 +915,26 @@
         <v>5</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(C:C,F11)</f>
         <v>1</v>
       </c>
       <c r="I11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <f>VLOOKUP(C12,F:F:G:G,2,FALSE)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -933,29 +943,29 @@
         <v>6</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(C:C,F12)</f>
         <v>3</v>
       </c>
       <c r="I12" t="s">
         <v>56</v>
       </c>
       <c r="J12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D13">
         <f>VLOOKUP(C13,F:F:G:G,2,FALSE)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13" t="s">
         <v>58</v>
@@ -964,26 +974,29 @@
         <v>7</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(C:C,F13)</f>
         <v>2</v>
       </c>
       <c r="I13" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="M13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D14">
         <f>VLOOKUP(C14,F:F:G:G,2,FALSE)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F14" t="s">
         <v>63</v>
@@ -992,26 +1005,26 @@
         <v>8</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(C:C,F14)</f>
         <v>1</v>
       </c>
       <c r="I14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D15">
         <f>VLOOKUP(C15,F:F:G:G,2,FALSE)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F15" t="s">
         <v>54</v>
@@ -1020,26 +1033,26 @@
         <v>9</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(C:C,F15)</f>
         <v>8</v>
       </c>
       <c r="I15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D16">
         <f>VLOOKUP(C16,F:F:G:G,2,FALSE)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F16" t="s">
         <v>64</v>
@@ -1048,7 +1061,7 @@
         <v>10</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(C:C,F16)</f>
         <v>1</v>
       </c>
       <c r="I16" t="s">
@@ -1057,17 +1070,17 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D17">
         <f>VLOOKUP(C17,F:F:G:G,2,FALSE)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
@@ -1076,17 +1089,17 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D18">
         <f>VLOOKUP(C18,F:F:G:G,2,FALSE)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -1095,17 +1108,14 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D19">
         <f>VLOOKUP(C19,F:F:G:G,2,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="9"/>
@@ -1114,17 +1124,17 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B20">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="D20">
         <f>VLOOKUP(C20,F:F:G:G,2,FALSE)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="8"/>
@@ -1133,17 +1143,17 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B21">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="D21">
         <f>VLOOKUP(C21,F:F:G:G,2,FALSE)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -1152,20 +1162,17 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B22">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" t="e">
+        <v>58</v>
+      </c>
+      <c r="D22">
         <f>VLOOKUP(C22,F:F:G:G,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E22" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -1174,17 +1181,17 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B23">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23">
         <f>VLOOKUP(C23,F:F:G:G,2,FALSE)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -1193,14 +1200,17 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>44</v>
+      </c>
+      <c r="B24">
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="D24">
         <f>VLOOKUP(C24,F:F:G:G,2,FALSE)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -1209,17 +1219,17 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B25">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="D25">
         <f>VLOOKUP(C25,F:F:G:G,2,FALSE)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -1228,17 +1238,17 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B26">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="D26">
         <f>VLOOKUP(C26,F:F:G:G,2,FALSE)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -1247,122 +1257,125 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="D27">
         <f>VLOOKUP(C27,F:F:G:G,2,FALSE)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B28">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="D28">
         <f>VLOOKUP(C28,F:F:G:G,2,FALSE)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B29">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="D29">
         <f>VLOOKUP(C29,F:F:G:G,2,FALSE)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30">
         <v>22</v>
       </c>
-      <c r="B30">
-        <v>12</v>
-      </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="D30">
         <f>VLOOKUP(C30,F:F:G:G,2,FALSE)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B31">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="D31">
         <f>VLOOKUP(C31,F:F:G:G,2,FALSE)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="D32">
         <f>VLOOKUP(C32,F:F:G:G,2,FALSE)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B33">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="D33">
         <f>VLOOKUP(C33,F:F:G:G,2,FALSE)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34">
+        <v>48</v>
+      </c>
+      <c r="D34" t="e">
         <f>VLOOKUP(C34,F:F:G:G,2,FALSE)</f>
-        <v>8</v>
+        <v>#N/A</v>
+      </c>
+      <c r="E34" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
@@ -1371,6 +1384,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E34">
+    <sortCondition ref="D2:D34"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>